<commit_message>
updating results excel sheet
</commit_message>
<xml_diff>
--- a/Python/2. Data Processing/2. Data Analysis/Initial_model_accuracy_results.xlsx
+++ b/Python/2. Data Processing/2. Data Analysis/Initial_model_accuracy_results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\2. Data Processing\2. Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72BF4AE-755A-4D72-BBA0-7591B8F7102C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A59E93-1CC9-4870-80B0-3A467EC14181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{96ABA9FB-0DD9-458B-8A8D-B7C9E47C7F0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{96ABA9FB-0DD9-458B-8A8D-B7C9E47C7F0D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BinarySearch" sheetId="1" r:id="rId1"/>
+    <sheet name="GridSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="26">
   <si>
     <t>Train</t>
   </si>
@@ -129,7 +130,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -424,27 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,8 +439,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -481,6 +467,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,7 +491,40 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -508,6 +542,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>105385</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D821125E-0EDA-F3E1-9575-C5DF2487B460}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10391775" y="390525"/>
+          <a:ext cx="4372585" cy="1638529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>589788</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>151829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EEE6FC7-E7FB-DE38-8B94-CB8AACF2B941}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181100" y="1905000"/>
+          <a:ext cx="6095238" cy="4571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69AEB7B-7BE9-4B9B-B207-ED55F3C9E6A2}">
   <dimension ref="B2:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,32 +947,32 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="43"/>
+      <c r="I3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="22" t="s">
+      <c r="J3" s="43"/>
+      <c r="K3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="23"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="21"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1066,120 +1193,120 @@
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="43"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="41"/>
     </row>
     <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="24" t="s">
+      <c r="D18" s="43"/>
+      <c r="E18" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="24" t="s">
+      <c r="F18" s="43"/>
+      <c r="G18" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="24" t="s">
+      <c r="H18" s="43"/>
+      <c r="I18" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="24" t="s">
+      <c r="J18" s="43"/>
+      <c r="K18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="24" t="s">
+      <c r="L18" s="43"/>
+      <c r="M18" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="25"/>
-      <c r="O18" s="24" t="s">
+      <c r="N18" s="43"/>
+      <c r="O18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="24" t="s">
+      <c r="P18" s="43"/>
+      <c r="Q18" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="25"/>
-      <c r="S18" s="24" t="s">
+      <c r="R18" s="43"/>
+      <c r="S18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="T18" s="25"/>
+      <c r="T18" s="43"/>
     </row>
     <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="26"/>
-      <c r="C19" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="40" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="40" t="s">
+      <c r="I19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K19" s="40" t="s">
+      <c r="K19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O19" s="40" t="s">
+      <c r="O19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q19" s="40" t="s">
+      <c r="Q19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S19" s="40" t="s">
+      <c r="S19" s="33" t="s">
         <v>0</v>
       </c>
       <c r="T19" s="4" t="s">
@@ -1187,117 +1314,117 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="30">
         <v>77</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="21">
         <v>77</v>
       </c>
-      <c r="E20" s="37">
-        <v>100</v>
-      </c>
-      <c r="F20" s="28">
-        <v>100</v>
-      </c>
-      <c r="G20" s="37">
-        <v>100</v>
-      </c>
-      <c r="H20" s="28">
-        <v>100</v>
-      </c>
-      <c r="I20" s="37">
-        <v>100</v>
-      </c>
-      <c r="J20" s="28">
-        <v>100</v>
-      </c>
-      <c r="K20" s="37">
-        <v>100</v>
-      </c>
-      <c r="L20" s="28">
-        <v>100</v>
-      </c>
-      <c r="M20" s="37">
-        <v>100</v>
-      </c>
-      <c r="N20" s="28">
-        <v>100</v>
-      </c>
-      <c r="O20" s="37">
-        <v>100</v>
-      </c>
-      <c r="P20" s="28">
-        <v>100</v>
-      </c>
-      <c r="Q20" s="37">
-        <v>100</v>
-      </c>
-      <c r="R20" s="28">
-        <v>100</v>
-      </c>
-      <c r="S20" s="37">
-        <v>100</v>
-      </c>
-      <c r="T20" s="28">
+      <c r="E20" s="30">
+        <v>100</v>
+      </c>
+      <c r="F20" s="21">
+        <v>100</v>
+      </c>
+      <c r="G20" s="30">
+        <v>100</v>
+      </c>
+      <c r="H20" s="21">
+        <v>100</v>
+      </c>
+      <c r="I20" s="30">
+        <v>100</v>
+      </c>
+      <c r="J20" s="21">
+        <v>100</v>
+      </c>
+      <c r="K20" s="30">
+        <v>100</v>
+      </c>
+      <c r="L20" s="21">
+        <v>100</v>
+      </c>
+      <c r="M20" s="30">
+        <v>100</v>
+      </c>
+      <c r="N20" s="21">
+        <v>100</v>
+      </c>
+      <c r="O20" s="30">
+        <v>100</v>
+      </c>
+      <c r="P20" s="21">
+        <v>100</v>
+      </c>
+      <c r="Q20" s="30">
+        <v>100</v>
+      </c>
+      <c r="R20" s="21">
+        <v>100</v>
+      </c>
+      <c r="S20" s="30">
+        <v>100</v>
+      </c>
+      <c r="T20" s="21">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="31">
         <v>100</v>
       </c>
       <c r="D21" s="7">
         <v>100</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="31">
         <v>100</v>
       </c>
       <c r="F21" s="7">
         <v>100</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="31">
         <v>100</v>
       </c>
       <c r="H21" s="7">
         <v>100</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="31">
         <v>100</v>
       </c>
       <c r="J21" s="7">
         <v>100</v>
       </c>
-      <c r="K21" s="38">
+      <c r="K21" s="31">
         <v>100</v>
       </c>
       <c r="L21" s="7">
         <v>100</v>
       </c>
-      <c r="M21" s="38">
+      <c r="M21" s="31">
         <v>100</v>
       </c>
       <c r="N21" s="7">
         <v>100</v>
       </c>
-      <c r="O21" s="38">
+      <c r="O21" s="31">
         <v>100</v>
       </c>
       <c r="P21" s="7">
         <v>100</v>
       </c>
-      <c r="Q21" s="38">
+      <c r="Q21" s="31">
         <v>100</v>
       </c>
       <c r="R21" s="7">
         <v>100</v>
       </c>
-      <c r="S21" s="38">
+      <c r="S21" s="31">
         <v>100</v>
       </c>
       <c r="T21" s="7">
@@ -1305,58 +1432,58 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="31">
         <v>100</v>
       </c>
       <c r="D22" s="7">
         <v>100</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="31">
         <v>100</v>
       </c>
       <c r="F22" s="7">
         <v>100</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="31">
         <v>100</v>
       </c>
       <c r="H22" s="7">
         <v>100</v>
       </c>
-      <c r="I22" s="38">
+      <c r="I22" s="31">
         <v>100</v>
       </c>
       <c r="J22" s="7">
         <v>100</v>
       </c>
-      <c r="K22" s="38">
+      <c r="K22" s="31">
         <v>100</v>
       </c>
       <c r="L22" s="7">
         <v>100</v>
       </c>
-      <c r="M22" s="38">
+      <c r="M22" s="31">
         <v>100</v>
       </c>
       <c r="N22" s="7">
         <v>100</v>
       </c>
-      <c r="O22" s="38">
+      <c r="O22" s="31">
         <v>100</v>
       </c>
       <c r="P22" s="7">
         <v>100</v>
       </c>
-      <c r="Q22" s="38">
+      <c r="Q22" s="31">
         <v>100</v>
       </c>
       <c r="R22" s="7">
         <v>100</v>
       </c>
-      <c r="S22" s="38">
+      <c r="S22" s="31">
         <v>100</v>
       </c>
       <c r="T22" s="7">
@@ -1364,58 +1491,58 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="31">
         <v>72</v>
       </c>
       <c r="D23" s="7">
         <v>72</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="31">
         <v>100</v>
       </c>
       <c r="F23" s="7">
         <v>100</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="31">
         <v>100</v>
       </c>
       <c r="H23" s="7">
         <v>100</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="31">
         <v>100</v>
       </c>
       <c r="J23" s="7">
         <v>100</v>
       </c>
-      <c r="K23" s="38">
+      <c r="K23" s="31">
         <v>100</v>
       </c>
       <c r="L23" s="7">
         <v>100</v>
       </c>
-      <c r="M23" s="38">
+      <c r="M23" s="31">
         <v>100</v>
       </c>
       <c r="N23" s="7">
         <v>100</v>
       </c>
-      <c r="O23" s="38">
+      <c r="O23" s="31">
         <v>100</v>
       </c>
       <c r="P23" s="7">
         <v>100</v>
       </c>
-      <c r="Q23" s="38">
+      <c r="Q23" s="31">
         <v>100</v>
       </c>
       <c r="R23" s="7">
         <v>100</v>
       </c>
-      <c r="S23" s="38">
+      <c r="S23" s="31">
         <v>100</v>
       </c>
       <c r="T23" s="7">
@@ -1423,58 +1550,58 @@
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="31">
         <v>81</v>
       </c>
       <c r="D24" s="7">
         <v>81</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="31">
         <v>100</v>
       </c>
       <c r="F24" s="7">
         <v>100</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="31">
         <v>100</v>
       </c>
       <c r="H24" s="7">
         <v>100</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="31">
         <v>100</v>
       </c>
       <c r="J24" s="7">
         <v>100</v>
       </c>
-      <c r="K24" s="38">
+      <c r="K24" s="31">
         <v>100</v>
       </c>
       <c r="L24" s="7">
         <v>100</v>
       </c>
-      <c r="M24" s="38">
+      <c r="M24" s="31">
         <v>100</v>
       </c>
       <c r="N24" s="7">
         <v>100</v>
       </c>
-      <c r="O24" s="38">
+      <c r="O24" s="31">
         <v>100</v>
       </c>
       <c r="P24" s="7">
         <v>100</v>
       </c>
-      <c r="Q24" s="38">
+      <c r="Q24" s="31">
         <v>100</v>
       </c>
       <c r="R24" s="7">
         <v>100</v>
       </c>
-      <c r="S24" s="38">
+      <c r="S24" s="31">
         <v>100</v>
       </c>
       <c r="T24" s="7">
@@ -1482,58 +1609,58 @@
       </c>
     </row>
     <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="32">
         <v>95</v>
       </c>
       <c r="D25" s="10">
         <v>95</v>
       </c>
-      <c r="E25" s="39">
+      <c r="E25" s="32">
         <v>100</v>
       </c>
       <c r="F25" s="10">
         <v>100</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="32">
         <v>100</v>
       </c>
       <c r="H25" s="10">
         <v>100</v>
       </c>
-      <c r="I25" s="39">
+      <c r="I25" s="32">
         <v>100</v>
       </c>
       <c r="J25" s="10">
         <v>100</v>
       </c>
-      <c r="K25" s="39">
+      <c r="K25" s="32">
         <v>100</v>
       </c>
       <c r="L25" s="10">
         <v>100</v>
       </c>
-      <c r="M25" s="39">
+      <c r="M25" s="32">
         <v>100</v>
       </c>
       <c r="N25" s="10">
         <v>100</v>
       </c>
-      <c r="O25" s="39">
+      <c r="O25" s="32">
         <v>100</v>
       </c>
       <c r="P25" s="10">
         <v>100</v>
       </c>
-      <c r="Q25" s="39">
+      <c r="Q25" s="32">
         <v>100</v>
       </c>
       <c r="R25" s="10">
         <v>100</v>
       </c>
-      <c r="S25" s="39">
+      <c r="S25" s="32">
         <v>100</v>
       </c>
       <c r="T25" s="10">
@@ -1542,120 +1669,120 @@
     </row>
     <row r="27" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="43"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="41"/>
     </row>
     <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="24" t="s">
+      <c r="D29" s="43"/>
+      <c r="E29" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="24" t="s">
+      <c r="F29" s="43"/>
+      <c r="G29" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="24" t="s">
+      <c r="H29" s="43"/>
+      <c r="I29" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="25"/>
-      <c r="K29" s="24" t="s">
+      <c r="J29" s="43"/>
+      <c r="K29" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="25"/>
-      <c r="M29" s="24" t="s">
+      <c r="L29" s="43"/>
+      <c r="M29" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="N29" s="25"/>
-      <c r="O29" s="24" t="s">
+      <c r="N29" s="43"/>
+      <c r="O29" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="24" t="s">
+      <c r="P29" s="43"/>
+      <c r="Q29" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="R29" s="25"/>
-      <c r="S29" s="24" t="s">
+      <c r="R29" s="43"/>
+      <c r="S29" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="T29" s="25"/>
+      <c r="T29" s="43"/>
     </row>
     <row r="30" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="26"/>
-      <c r="C30" s="40" t="s">
+      <c r="B30" s="38"/>
+      <c r="C30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="40" t="s">
+      <c r="K30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M30" s="40" t="s">
+      <c r="M30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O30" s="40" t="s">
+      <c r="O30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="P30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q30" s="40" t="s">
+      <c r="Q30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S30" s="40" t="s">
+      <c r="S30" s="33" t="s">
         <v>0</v>
       </c>
       <c r="T30" s="4" t="s">
@@ -1663,117 +1790,117 @@
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="37">
-        <v>100</v>
-      </c>
-      <c r="D31" s="28">
-        <v>100</v>
-      </c>
-      <c r="E31" s="37">
-        <v>100</v>
-      </c>
-      <c r="F31" s="28">
-        <v>100</v>
-      </c>
-      <c r="G31" s="37">
-        <v>100</v>
-      </c>
-      <c r="H31" s="28">
-        <v>100</v>
-      </c>
-      <c r="I31" s="37">
-        <v>100</v>
-      </c>
-      <c r="J31" s="28">
-        <v>100</v>
-      </c>
-      <c r="K31" s="37">
-        <v>100</v>
-      </c>
-      <c r="L31" s="28">
-        <v>100</v>
-      </c>
-      <c r="M31" s="37">
-        <v>100</v>
-      </c>
-      <c r="N31" s="28">
-        <v>100</v>
-      </c>
-      <c r="O31" s="37">
-        <v>100</v>
-      </c>
-      <c r="P31" s="28">
-        <v>100</v>
-      </c>
-      <c r="Q31" s="37">
-        <v>100</v>
-      </c>
-      <c r="R31" s="28">
-        <v>100</v>
-      </c>
-      <c r="S31" s="37">
-        <v>100</v>
-      </c>
-      <c r="T31" s="28">
+      <c r="C31" s="30">
+        <v>100</v>
+      </c>
+      <c r="D31" s="21">
+        <v>100</v>
+      </c>
+      <c r="E31" s="30">
+        <v>100</v>
+      </c>
+      <c r="F31" s="21">
+        <v>100</v>
+      </c>
+      <c r="G31" s="30">
+        <v>100</v>
+      </c>
+      <c r="H31" s="21">
+        <v>100</v>
+      </c>
+      <c r="I31" s="30">
+        <v>100</v>
+      </c>
+      <c r="J31" s="21">
+        <v>100</v>
+      </c>
+      <c r="K31" s="30">
+        <v>100</v>
+      </c>
+      <c r="L31" s="21">
+        <v>100</v>
+      </c>
+      <c r="M31" s="30">
+        <v>100</v>
+      </c>
+      <c r="N31" s="21">
+        <v>100</v>
+      </c>
+      <c r="O31" s="30">
+        <v>100</v>
+      </c>
+      <c r="P31" s="21">
+        <v>100</v>
+      </c>
+      <c r="Q31" s="30">
+        <v>100</v>
+      </c>
+      <c r="R31" s="21">
+        <v>100</v>
+      </c>
+      <c r="S31" s="30">
+        <v>100</v>
+      </c>
+      <c r="T31" s="21">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="31">
         <v>100</v>
       </c>
       <c r="D32" s="7">
         <v>100</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="31">
         <v>100</v>
       </c>
       <c r="F32" s="7">
         <v>100</v>
       </c>
-      <c r="G32" s="38">
+      <c r="G32" s="31">
         <v>100</v>
       </c>
       <c r="H32" s="7">
         <v>100</v>
       </c>
-      <c r="I32" s="38">
+      <c r="I32" s="31">
         <v>100</v>
       </c>
       <c r="J32" s="7">
         <v>100</v>
       </c>
-      <c r="K32" s="38">
+      <c r="K32" s="31">
         <v>100</v>
       </c>
       <c r="L32" s="7">
         <v>100</v>
       </c>
-      <c r="M32" s="38">
+      <c r="M32" s="31">
         <v>100</v>
       </c>
       <c r="N32" s="7">
         <v>100</v>
       </c>
-      <c r="O32" s="38">
+      <c r="O32" s="31">
         <v>100</v>
       </c>
       <c r="P32" s="7">
         <v>100</v>
       </c>
-      <c r="Q32" s="38">
+      <c r="Q32" s="31">
         <v>100</v>
       </c>
       <c r="R32" s="7">
         <v>100</v>
       </c>
-      <c r="S32" s="38">
+      <c r="S32" s="31">
         <v>100</v>
       </c>
       <c r="T32" s="7">
@@ -1781,58 +1908,58 @@
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="31">
         <v>100</v>
       </c>
       <c r="D33" s="7">
         <v>100</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="31">
         <v>100</v>
       </c>
       <c r="F33" s="7">
         <v>100</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="31">
         <v>100</v>
       </c>
       <c r="H33" s="7">
         <v>100</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="31">
         <v>100</v>
       </c>
       <c r="J33" s="7">
         <v>100</v>
       </c>
-      <c r="K33" s="38">
+      <c r="K33" s="31">
         <v>100</v>
       </c>
       <c r="L33" s="7">
         <v>100</v>
       </c>
-      <c r="M33" s="38">
+      <c r="M33" s="31">
         <v>100</v>
       </c>
       <c r="N33" s="7">
         <v>100</v>
       </c>
-      <c r="O33" s="38">
+      <c r="O33" s="31">
         <v>100</v>
       </c>
       <c r="P33" s="7">
         <v>100</v>
       </c>
-      <c r="Q33" s="38">
+      <c r="Q33" s="31">
         <v>100</v>
       </c>
       <c r="R33" s="7">
         <v>100</v>
       </c>
-      <c r="S33" s="38">
+      <c r="S33" s="31">
         <v>100</v>
       </c>
       <c r="T33" s="7">
@@ -1840,58 +1967,58 @@
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="31">
         <v>100</v>
       </c>
       <c r="D34" s="7">
         <v>100</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="31">
         <v>100</v>
       </c>
       <c r="F34" s="7">
         <v>100</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="31">
         <v>100</v>
       </c>
       <c r="H34" s="7">
         <v>100</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="31">
         <v>100</v>
       </c>
       <c r="J34" s="7">
         <v>100</v>
       </c>
-      <c r="K34" s="38">
+      <c r="K34" s="31">
         <v>100</v>
       </c>
       <c r="L34" s="7">
         <v>100</v>
       </c>
-      <c r="M34" s="38">
+      <c r="M34" s="31">
         <v>100</v>
       </c>
       <c r="N34" s="7">
         <v>100</v>
       </c>
-      <c r="O34" s="38">
+      <c r="O34" s="31">
         <v>100</v>
       </c>
       <c r="P34" s="7">
         <v>100</v>
       </c>
-      <c r="Q34" s="38">
+      <c r="Q34" s="31">
         <v>100</v>
       </c>
       <c r="R34" s="7">
         <v>100</v>
       </c>
-      <c r="S34" s="38">
+      <c r="S34" s="31">
         <v>100</v>
       </c>
       <c r="T34" s="7">
@@ -1899,58 +2026,58 @@
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="31">
         <v>100</v>
       </c>
       <c r="D35" s="7">
         <v>100</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="31">
         <v>100</v>
       </c>
       <c r="F35" s="7">
         <v>100</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="31">
         <v>100</v>
       </c>
       <c r="H35" s="7">
         <v>100</v>
       </c>
-      <c r="I35" s="38">
+      <c r="I35" s="31">
         <v>100</v>
       </c>
       <c r="J35" s="7">
         <v>100</v>
       </c>
-      <c r="K35" s="38">
+      <c r="K35" s="31">
         <v>100</v>
       </c>
       <c r="L35" s="7">
         <v>100</v>
       </c>
-      <c r="M35" s="38">
+      <c r="M35" s="31">
         <v>100</v>
       </c>
       <c r="N35" s="7">
         <v>100</v>
       </c>
-      <c r="O35" s="38">
+      <c r="O35" s="31">
         <v>100</v>
       </c>
       <c r="P35" s="7">
         <v>100</v>
       </c>
-      <c r="Q35" s="38">
+      <c r="Q35" s="31">
         <v>100</v>
       </c>
       <c r="R35" s="7">
         <v>100</v>
       </c>
-      <c r="S35" s="38">
+      <c r="S35" s="31">
         <v>100</v>
       </c>
       <c r="T35" s="7">
@@ -1958,58 +2085,58 @@
       </c>
     </row>
     <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="39">
+      <c r="C36" s="32">
         <v>100</v>
       </c>
       <c r="D36" s="10">
         <v>100</v>
       </c>
-      <c r="E36" s="39">
+      <c r="E36" s="32">
         <v>100</v>
       </c>
       <c r="F36" s="10">
         <v>100</v>
       </c>
-      <c r="G36" s="39">
+      <c r="G36" s="32">
         <v>100</v>
       </c>
       <c r="H36" s="10">
         <v>100</v>
       </c>
-      <c r="I36" s="39">
+      <c r="I36" s="32">
         <v>100</v>
       </c>
       <c r="J36" s="10">
         <v>100</v>
       </c>
-      <c r="K36" s="39">
+      <c r="K36" s="32">
         <v>100</v>
       </c>
       <c r="L36" s="10">
         <v>100</v>
       </c>
-      <c r="M36" s="39">
+      <c r="M36" s="32">
         <v>100</v>
       </c>
       <c r="N36" s="10">
         <v>100</v>
       </c>
-      <c r="O36" s="39">
+      <c r="O36" s="32">
         <v>100</v>
       </c>
       <c r="P36" s="10">
         <v>100</v>
       </c>
-      <c r="Q36" s="39">
+      <c r="Q36" s="32">
         <v>100</v>
       </c>
       <c r="R36" s="10">
         <v>100</v>
       </c>
-      <c r="S36" s="39">
+      <c r="S36" s="32">
         <v>100</v>
       </c>
       <c r="T36" s="10">
@@ -2018,114 +2145,114 @@
     </row>
     <row r="38" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="42"/>
-      <c r="L39" s="42"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="42"/>
-      <c r="Q39" s="42"/>
-      <c r="R39" s="42"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="43"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="40"/>
+      <c r="Q39" s="40"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="41"/>
     </row>
     <row r="40" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="24" t="s">
+      <c r="D40" s="43"/>
+      <c r="E40" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="24" t="s">
+      <c r="F40" s="43"/>
+      <c r="G40" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="24" t="s">
+      <c r="H40" s="43"/>
+      <c r="I40" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="J40" s="25"/>
-      <c r="K40" s="24" t="s">
+      <c r="J40" s="43"/>
+      <c r="K40" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="25"/>
-      <c r="M40" s="24" t="s">
+      <c r="L40" s="43"/>
+      <c r="M40" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="N40" s="25"/>
-      <c r="O40" s="24" t="s">
+      <c r="N40" s="43"/>
+      <c r="O40" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="25"/>
-      <c r="Q40" s="24" t="s">
+      <c r="P40" s="43"/>
+      <c r="Q40" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="R40" s="25"/>
-      <c r="S40" s="24" t="s">
+      <c r="R40" s="43"/>
+      <c r="S40" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="T40" s="25"/>
+      <c r="T40" s="43"/>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="26"/>
-      <c r="C41" s="40" t="s">
+      <c r="B41" s="38"/>
+      <c r="C41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G41" s="40" t="s">
+      <c r="G41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I41" s="40" t="s">
+      <c r="I41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K41" s="40" t="s">
+      <c r="K41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M41" s="40" t="s">
+      <c r="M41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O41" s="40" t="s">
+      <c r="O41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="P41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Q41" s="40" t="s">
+      <c r="Q41" s="33" t="s">
         <v>0</v>
       </c>
       <c r="R41" s="4" t="s">
@@ -2139,117 +2266,117 @@
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="37">
-        <v>100</v>
-      </c>
-      <c r="D42" s="28">
-        <v>100</v>
-      </c>
-      <c r="E42" s="37">
-        <v>100</v>
-      </c>
-      <c r="F42" s="28">
-        <v>100</v>
-      </c>
-      <c r="G42" s="37">
-        <v>100</v>
-      </c>
-      <c r="H42" s="28">
-        <v>100</v>
-      </c>
-      <c r="I42" s="37">
+      <c r="C42" s="30">
+        <v>100</v>
+      </c>
+      <c r="D42" s="21">
+        <v>100</v>
+      </c>
+      <c r="E42" s="30">
+        <v>100</v>
+      </c>
+      <c r="F42" s="21">
+        <v>100</v>
+      </c>
+      <c r="G42" s="30">
+        <v>100</v>
+      </c>
+      <c r="H42" s="21">
+        <v>100</v>
+      </c>
+      <c r="I42" s="30">
         <v>97</v>
       </c>
-      <c r="J42" s="28">
+      <c r="J42" s="21">
         <v>97</v>
       </c>
-      <c r="K42" s="37">
-        <v>100</v>
-      </c>
-      <c r="L42" s="28">
-        <v>100</v>
-      </c>
-      <c r="M42" s="37">
-        <v>100</v>
-      </c>
-      <c r="N42" s="28">
-        <v>100</v>
-      </c>
-      <c r="O42" s="37">
-        <v>100</v>
-      </c>
-      <c r="P42" s="28">
-        <v>100</v>
-      </c>
-      <c r="Q42" s="37">
-        <v>100</v>
-      </c>
-      <c r="R42" s="28">
-        <v>100</v>
-      </c>
-      <c r="S42" s="37">
-        <v>100</v>
-      </c>
-      <c r="T42" s="28">
+      <c r="K42" s="30">
+        <v>100</v>
+      </c>
+      <c r="L42" s="21">
+        <v>100</v>
+      </c>
+      <c r="M42" s="30">
+        <v>100</v>
+      </c>
+      <c r="N42" s="21">
+        <v>100</v>
+      </c>
+      <c r="O42" s="30">
+        <v>100</v>
+      </c>
+      <c r="P42" s="21">
+        <v>100</v>
+      </c>
+      <c r="Q42" s="30">
+        <v>100</v>
+      </c>
+      <c r="R42" s="21">
+        <v>100</v>
+      </c>
+      <c r="S42" s="30">
+        <v>100</v>
+      </c>
+      <c r="T42" s="21">
         <v>100</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="38">
+      <c r="C43" s="31">
         <v>100</v>
       </c>
       <c r="D43" s="7">
         <v>100</v>
       </c>
-      <c r="E43" s="38">
+      <c r="E43" s="31">
         <v>100</v>
       </c>
       <c r="F43" s="7">
         <v>100</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="31">
         <v>100</v>
       </c>
       <c r="H43" s="7">
         <v>100</v>
       </c>
-      <c r="I43" s="38">
+      <c r="I43" s="31">
         <v>100</v>
       </c>
       <c r="J43" s="7">
         <v>100</v>
       </c>
-      <c r="K43" s="38">
+      <c r="K43" s="31">
         <v>100</v>
       </c>
       <c r="L43" s="7">
         <v>100</v>
       </c>
-      <c r="M43" s="38">
+      <c r="M43" s="31">
         <v>100</v>
       </c>
       <c r="N43" s="7">
         <v>100</v>
       </c>
-      <c r="O43" s="38">
+      <c r="O43" s="31">
         <v>100</v>
       </c>
       <c r="P43" s="7">
         <v>100</v>
       </c>
-      <c r="Q43" s="38">
+      <c r="Q43" s="31">
         <v>100</v>
       </c>
       <c r="R43" s="7">
         <v>100</v>
       </c>
-      <c r="S43" s="38">
+      <c r="S43" s="31">
         <v>100</v>
       </c>
       <c r="T43" s="7">
@@ -2257,58 +2384,58 @@
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="38">
+      <c r="C44" s="31">
         <v>100</v>
       </c>
       <c r="D44" s="7">
         <v>100</v>
       </c>
-      <c r="E44" s="38">
+      <c r="E44" s="31">
         <v>100</v>
       </c>
       <c r="F44" s="7">
         <v>100</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="31">
         <v>100</v>
       </c>
       <c r="H44" s="7">
         <v>100</v>
       </c>
-      <c r="I44" s="38">
+      <c r="I44" s="31">
         <v>100</v>
       </c>
       <c r="J44" s="7">
         <v>100</v>
       </c>
-      <c r="K44" s="38">
+      <c r="K44" s="31">
         <v>100</v>
       </c>
       <c r="L44" s="7">
         <v>100</v>
       </c>
-      <c r="M44" s="38">
+      <c r="M44" s="31">
         <v>100</v>
       </c>
       <c r="N44" s="7">
         <v>100</v>
       </c>
-      <c r="O44" s="38">
+      <c r="O44" s="31">
         <v>100</v>
       </c>
       <c r="P44" s="7">
         <v>100</v>
       </c>
-      <c r="Q44" s="38">
+      <c r="Q44" s="31">
         <v>100</v>
       </c>
       <c r="R44" s="7">
         <v>100</v>
       </c>
-      <c r="S44" s="38">
+      <c r="S44" s="31">
         <v>100</v>
       </c>
       <c r="T44" s="7">
@@ -2316,58 +2443,58 @@
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="38">
+      <c r="C45" s="31">
         <v>100</v>
       </c>
       <c r="D45" s="7">
         <v>100</v>
       </c>
-      <c r="E45" s="38">
+      <c r="E45" s="31">
         <v>100</v>
       </c>
       <c r="F45" s="7">
         <v>100</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="31">
         <v>100</v>
       </c>
       <c r="H45" s="7">
         <v>100</v>
       </c>
-      <c r="I45" s="38">
+      <c r="I45" s="31">
         <v>98</v>
       </c>
       <c r="J45" s="7">
         <v>97</v>
       </c>
-      <c r="K45" s="38">
+      <c r="K45" s="31">
         <v>100</v>
       </c>
       <c r="L45" s="7">
         <v>100</v>
       </c>
-      <c r="M45" s="38">
+      <c r="M45" s="31">
         <v>100</v>
       </c>
       <c r="N45" s="7">
         <v>100</v>
       </c>
-      <c r="O45" s="38">
+      <c r="O45" s="31">
         <v>100</v>
       </c>
       <c r="P45" s="7">
         <v>100</v>
       </c>
-      <c r="Q45" s="38">
+      <c r="Q45" s="31">
         <v>100</v>
       </c>
       <c r="R45" s="7">
         <v>100</v>
       </c>
-      <c r="S45" s="38">
+      <c r="S45" s="31">
         <v>100</v>
       </c>
       <c r="T45" s="7">
@@ -2375,58 +2502,58 @@
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="38">
+      <c r="C46" s="31">
         <v>100</v>
       </c>
       <c r="D46" s="7">
         <v>100</v>
       </c>
-      <c r="E46" s="38">
+      <c r="E46" s="31">
         <v>100</v>
       </c>
       <c r="F46" s="7">
         <v>100</v>
       </c>
-      <c r="G46" s="38">
+      <c r="G46" s="31">
         <v>100</v>
       </c>
       <c r="H46" s="7">
         <v>100</v>
       </c>
-      <c r="I46" s="38">
+      <c r="I46" s="31">
         <v>99</v>
       </c>
       <c r="J46" s="7">
         <v>99</v>
       </c>
-      <c r="K46" s="38">
+      <c r="K46" s="31">
         <v>100</v>
       </c>
       <c r="L46" s="7">
         <v>100</v>
       </c>
-      <c r="M46" s="38">
+      <c r="M46" s="31">
         <v>100</v>
       </c>
       <c r="N46" s="7">
         <v>100</v>
       </c>
-      <c r="O46" s="38">
+      <c r="O46" s="31">
         <v>100</v>
       </c>
       <c r="P46" s="7">
         <v>100</v>
       </c>
-      <c r="Q46" s="38">
+      <c r="Q46" s="31">
         <v>100</v>
       </c>
       <c r="R46" s="7">
         <v>100</v>
       </c>
-      <c r="S46" s="38">
+      <c r="S46" s="31">
         <v>100</v>
       </c>
       <c r="T46" s="7">
@@ -2434,58 +2561,58 @@
       </c>
     </row>
     <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="39">
+      <c r="C47" s="32">
         <v>100</v>
       </c>
       <c r="D47" s="10">
         <v>100</v>
       </c>
-      <c r="E47" s="39">
+      <c r="E47" s="32">
         <v>100</v>
       </c>
       <c r="F47" s="10">
         <v>100</v>
       </c>
-      <c r="G47" s="39">
+      <c r="G47" s="32">
         <v>100</v>
       </c>
       <c r="H47" s="10">
         <v>100</v>
       </c>
-      <c r="I47" s="39">
+      <c r="I47" s="32">
         <v>99</v>
       </c>
       <c r="J47" s="10">
         <v>99</v>
       </c>
-      <c r="K47" s="39">
+      <c r="K47" s="32">
         <v>100</v>
       </c>
       <c r="L47" s="10">
         <v>100</v>
       </c>
-      <c r="M47" s="39">
+      <c r="M47" s="32">
         <v>100</v>
       </c>
       <c r="N47" s="10">
         <v>100</v>
       </c>
-      <c r="O47" s="39">
+      <c r="O47" s="32">
         <v>100</v>
       </c>
       <c r="P47" s="10">
         <v>100</v>
       </c>
-      <c r="Q47" s="39">
+      <c r="Q47" s="32">
         <v>100</v>
       </c>
       <c r="R47" s="10">
         <v>100</v>
       </c>
-      <c r="S47" s="39">
+      <c r="S47" s="32">
         <v>100</v>
       </c>
       <c r="T47" s="10">
@@ -2494,71 +2621,71 @@
     </row>
     <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="42"/>
-      <c r="L50" s="42"/>
-      <c r="M50" s="42"/>
-      <c r="N50" s="42"/>
-      <c r="O50" s="42"/>
-      <c r="P50" s="42"/>
-      <c r="Q50" s="42"/>
-      <c r="R50" s="42"/>
-      <c r="S50" s="42"/>
-      <c r="T50" s="43"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="40"/>
+      <c r="N50" s="40"/>
+      <c r="O50" s="40"/>
+      <c r="P50" s="40"/>
+      <c r="Q50" s="40"/>
+      <c r="R50" s="40"/>
+      <c r="S50" s="40"/>
+      <c r="T50" s="41"/>
     </row>
     <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="24" t="s">
+      <c r="D51" s="43"/>
+      <c r="E51" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="25"/>
-      <c r="G51" s="24" t="s">
+      <c r="F51" s="43"/>
+      <c r="G51" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H51" s="25"/>
-      <c r="I51" s="24" t="s">
+      <c r="H51" s="43"/>
+      <c r="I51" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="J51" s="25"/>
-      <c r="K51" s="24" t="s">
+      <c r="J51" s="43"/>
+      <c r="K51" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L51" s="25"/>
-      <c r="M51" s="24" t="s">
+      <c r="L51" s="43"/>
+      <c r="M51" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="N51" s="25"/>
-      <c r="O51" s="24" t="s">
+      <c r="N51" s="43"/>
+      <c r="O51" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="P51" s="25"/>
-      <c r="Q51" s="24" t="s">
+      <c r="P51" s="43"/>
+      <c r="Q51" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="R51" s="25"/>
-      <c r="S51" s="24" t="s">
+      <c r="R51" s="43"/>
+      <c r="S51" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="T51" s="25"/>
+      <c r="T51" s="43"/>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="26"/>
+      <c r="B52" s="38"/>
       <c r="C52" s="3" t="s">
         <v>0</v>
       </c>
@@ -2615,66 +2742,66 @@
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="27">
-        <v>100</v>
-      </c>
-      <c r="D53" s="28">
-        <v>100</v>
-      </c>
-      <c r="E53" s="27">
-        <v>100</v>
-      </c>
-      <c r="F53" s="28">
-        <v>100</v>
-      </c>
-      <c r="G53" s="27">
-        <v>100</v>
-      </c>
-      <c r="H53" s="28">
-        <v>100</v>
-      </c>
-      <c r="I53" s="27">
-        <v>100</v>
-      </c>
-      <c r="J53" s="28">
-        <v>100</v>
-      </c>
-      <c r="K53" s="27">
-        <v>100</v>
-      </c>
-      <c r="L53" s="28">
-        <v>100</v>
-      </c>
-      <c r="M53" s="27">
-        <v>100</v>
-      </c>
-      <c r="N53" s="28">
-        <v>100</v>
-      </c>
-      <c r="O53" s="27">
-        <v>100</v>
-      </c>
-      <c r="P53" s="28">
-        <v>100</v>
-      </c>
-      <c r="Q53" s="27">
-        <v>100</v>
-      </c>
-      <c r="R53" s="28">
-        <v>100</v>
-      </c>
-      <c r="S53" s="27">
-        <v>100</v>
-      </c>
-      <c r="T53" s="28">
+      <c r="C53" s="20">
+        <v>100</v>
+      </c>
+      <c r="D53" s="21">
+        <v>100</v>
+      </c>
+      <c r="E53" s="20">
+        <v>100</v>
+      </c>
+      <c r="F53" s="21">
+        <v>100</v>
+      </c>
+      <c r="G53" s="20">
+        <v>100</v>
+      </c>
+      <c r="H53" s="21">
+        <v>100</v>
+      </c>
+      <c r="I53" s="20">
+        <v>100</v>
+      </c>
+      <c r="J53" s="21">
+        <v>100</v>
+      </c>
+      <c r="K53" s="20">
+        <v>100</v>
+      </c>
+      <c r="L53" s="21">
+        <v>100</v>
+      </c>
+      <c r="M53" s="20">
+        <v>100</v>
+      </c>
+      <c r="N53" s="21">
+        <v>100</v>
+      </c>
+      <c r="O53" s="20">
+        <v>100</v>
+      </c>
+      <c r="P53" s="21">
+        <v>100</v>
+      </c>
+      <c r="Q53" s="20">
+        <v>100</v>
+      </c>
+      <c r="R53" s="21">
+        <v>100</v>
+      </c>
+      <c r="S53" s="20">
+        <v>100</v>
+      </c>
+      <c r="T53" s="21">
         <v>100</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C54" s="6">
@@ -2733,7 +2860,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="6">
@@ -2792,7 +2919,7 @@
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="6">
@@ -2851,7 +2978,7 @@
       </c>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="6">
@@ -2910,7 +3037,7 @@
       </c>
     </row>
     <row r="58" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="9">
@@ -2969,71 +3096,71 @@
       </c>
     </row>
     <row r="61" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="44"/>
-      <c r="M61" s="44"/>
-      <c r="N61" s="44"/>
-      <c r="O61" s="44"/>
-      <c r="P61" s="44"/>
-      <c r="Q61" s="44"/>
-      <c r="R61" s="44"/>
-      <c r="S61" s="44"/>
-      <c r="T61" s="44"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="34"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="34"/>
+      <c r="O61" s="34"/>
+      <c r="P61" s="34"/>
+      <c r="Q61" s="34"/>
+      <c r="R61" s="34"/>
+      <c r="S61" s="34"/>
+      <c r="T61" s="34"/>
     </row>
     <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="23"/>
-      <c r="E62" s="22" t="s">
+      <c r="D62" s="36"/>
+      <c r="E62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="23"/>
-      <c r="G62" s="22" t="s">
+      <c r="F62" s="36"/>
+      <c r="G62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="23"/>
-      <c r="I62" s="22" t="s">
+      <c r="H62" s="36"/>
+      <c r="I62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J62" s="23"/>
-      <c r="K62" s="22" t="s">
+      <c r="J62" s="36"/>
+      <c r="K62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L62" s="23"/>
-      <c r="M62" s="22" t="s">
+      <c r="L62" s="36"/>
+      <c r="M62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="N62" s="23"/>
-      <c r="O62" s="22" t="s">
+      <c r="N62" s="36"/>
+      <c r="O62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="P62" s="23"/>
-      <c r="Q62" s="22" t="s">
+      <c r="P62" s="36"/>
+      <c r="Q62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="R62" s="23"/>
-      <c r="S62" s="22" t="s">
+      <c r="R62" s="36"/>
+      <c r="S62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="T62" s="23"/>
+      <c r="T62" s="36"/>
     </row>
     <row r="63" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="26"/>
+      <c r="B63" s="38"/>
       <c r="C63" s="12" t="s">
         <v>0</v>
       </c>
@@ -3090,69 +3217,69 @@
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="29" t="s">
+      <c r="B64" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="33">
+      <c r="C64" s="26">
         <v>61</v>
       </c>
-      <c r="D64" s="34">
+      <c r="D64" s="27">
         <v>61</v>
       </c>
-      <c r="E64" s="35">
-        <v>100</v>
-      </c>
-      <c r="F64" s="34">
-        <v>100</v>
-      </c>
-      <c r="G64" s="35">
-        <v>100</v>
-      </c>
-      <c r="H64" s="34">
-        <v>100</v>
-      </c>
-      <c r="I64" s="35">
-        <v>100</v>
-      </c>
-      <c r="J64" s="34">
-        <v>100</v>
-      </c>
-      <c r="K64" s="35">
-        <v>100</v>
-      </c>
-      <c r="L64" s="34">
-        <v>100</v>
-      </c>
-      <c r="M64" s="35">
+      <c r="E64" s="28">
+        <v>100</v>
+      </c>
+      <c r="F64" s="27">
+        <v>100</v>
+      </c>
+      <c r="G64" s="28">
+        <v>100</v>
+      </c>
+      <c r="H64" s="27">
+        <v>100</v>
+      </c>
+      <c r="I64" s="28">
+        <v>100</v>
+      </c>
+      <c r="J64" s="27">
+        <v>100</v>
+      </c>
+      <c r="K64" s="28">
+        <v>100</v>
+      </c>
+      <c r="L64" s="27">
+        <v>100</v>
+      </c>
+      <c r="M64" s="28">
         <v>95</v>
       </c>
-      <c r="N64" s="34">
+      <c r="N64" s="27">
         <v>95</v>
       </c>
-      <c r="O64" s="35">
-        <v>100</v>
-      </c>
-      <c r="P64" s="34">
-        <v>100</v>
-      </c>
-      <c r="Q64" s="35">
-        <v>100</v>
-      </c>
-      <c r="R64" s="34">
-        <v>100</v>
-      </c>
-      <c r="S64" s="35">
-        <v>100</v>
-      </c>
-      <c r="T64" s="34">
+      <c r="O64" s="28">
+        <v>100</v>
+      </c>
+      <c r="P64" s="27">
+        <v>100</v>
+      </c>
+      <c r="Q64" s="28">
+        <v>100</v>
+      </c>
+      <c r="R64" s="27">
+        <v>100</v>
+      </c>
+      <c r="S64" s="28">
+        <v>100</v>
+      </c>
+      <c r="T64" s="27">
         <v>100</v>
       </c>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="32">
+      <c r="C65" s="25">
         <v>98</v>
       </c>
       <c r="D65" s="15">
@@ -3208,10 +3335,10 @@
       </c>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="32">
+      <c r="C66" s="25">
         <v>97</v>
       </c>
       <c r="D66" s="15">
@@ -3267,10 +3394,10 @@
       </c>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="32">
+      <c r="C67" s="25">
         <v>61</v>
       </c>
       <c r="D67" s="15">
@@ -3326,10 +3453,10 @@
       </c>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="32">
+      <c r="C68" s="25">
         <v>79</v>
       </c>
       <c r="D68" s="15">
@@ -3385,10 +3512,10 @@
       </c>
     </row>
     <row r="69" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="36">
+      <c r="C69" s="29">
         <v>81</v>
       </c>
       <c r="D69" s="17">
@@ -3445,17 +3572,40 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="B61:T61"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="S62:T62"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B17:T17"/>
+    <mergeCell ref="B28:T28"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
     <mergeCell ref="B39:T39"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:D51"/>
@@ -3472,42 +3622,336 @@
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B17:T17"/>
-    <mergeCell ref="B28:T28"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B61:T61"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="S62:T62"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="I62:J62"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7590D5-C11D-488D-8E32-69EE70D35CC7}">
+  <dimension ref="B2:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="11" max="11" width="0.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="43"/>
+      <c r="I3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="43"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="44"/>
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="51"/>
+      <c r="L4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="45">
+        <v>80</v>
+      </c>
+      <c r="D5" s="46">
+        <v>80</v>
+      </c>
+      <c r="E5" s="45">
+        <v>99</v>
+      </c>
+      <c r="F5" s="46">
+        <v>99</v>
+      </c>
+      <c r="G5" s="45">
+        <v>97</v>
+      </c>
+      <c r="H5" s="46">
+        <v>97</v>
+      </c>
+      <c r="I5" s="47">
+        <v>96</v>
+      </c>
+      <c r="J5" s="46">
+        <v>96</v>
+      </c>
+      <c r="K5" s="52"/>
+      <c r="L5" s="45">
+        <v>93</v>
+      </c>
+      <c r="M5" s="46">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="45">
+        <v>100</v>
+      </c>
+      <c r="D6" s="46">
+        <v>100</v>
+      </c>
+      <c r="E6" s="45">
+        <v>100</v>
+      </c>
+      <c r="F6" s="46">
+        <v>100</v>
+      </c>
+      <c r="G6" s="45">
+        <v>100</v>
+      </c>
+      <c r="H6" s="46">
+        <v>100</v>
+      </c>
+      <c r="I6" s="47">
+        <v>100</v>
+      </c>
+      <c r="J6" s="46">
+        <v>100</v>
+      </c>
+      <c r="K6" s="52"/>
+      <c r="L6" s="45">
+        <v>100</v>
+      </c>
+      <c r="M6" s="46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="45">
+        <v>100</v>
+      </c>
+      <c r="D7" s="46">
+        <v>100</v>
+      </c>
+      <c r="E7" s="45">
+        <v>100</v>
+      </c>
+      <c r="F7" s="46">
+        <v>100</v>
+      </c>
+      <c r="G7" s="45">
+        <v>100</v>
+      </c>
+      <c r="H7" s="46">
+        <v>100</v>
+      </c>
+      <c r="I7" s="47">
+        <v>100</v>
+      </c>
+      <c r="J7" s="46">
+        <v>100</v>
+      </c>
+      <c r="K7" s="52"/>
+      <c r="L7" s="45">
+        <v>100</v>
+      </c>
+      <c r="M7" s="46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="45">
+        <v>66</v>
+      </c>
+      <c r="D8" s="46">
+        <v>65</v>
+      </c>
+      <c r="E8" s="45">
+        <v>97</v>
+      </c>
+      <c r="F8" s="46">
+        <v>97</v>
+      </c>
+      <c r="G8" s="45">
+        <v>96</v>
+      </c>
+      <c r="H8" s="46">
+        <v>96</v>
+      </c>
+      <c r="I8" s="47">
+        <v>95</v>
+      </c>
+      <c r="J8" s="46">
+        <v>95</v>
+      </c>
+      <c r="K8" s="52"/>
+      <c r="L8" s="45">
+        <v>95</v>
+      </c>
+      <c r="M8" s="46">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="48">
+        <v>91</v>
+      </c>
+      <c r="D9" s="49">
+        <v>91</v>
+      </c>
+      <c r="E9" s="48">
+        <v>100</v>
+      </c>
+      <c r="F9" s="49">
+        <v>100</v>
+      </c>
+      <c r="G9" s="48">
+        <v>99</v>
+      </c>
+      <c r="H9" s="49">
+        <v>99</v>
+      </c>
+      <c r="I9" s="50">
+        <v>99</v>
+      </c>
+      <c r="J9" s="49">
+        <v>100</v>
+      </c>
+      <c r="K9" s="53"/>
+      <c r="L9" s="48">
+        <v>97</v>
+      </c>
+      <c r="M9" s="49">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:J9">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L5:M9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:J9">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:M9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating results file with info showing models fall over
</commit_message>
<xml_diff>
--- a/Python/2. Data Processing/2. Data Analysis/Initial_model_accuracy_results.xlsx
+++ b/Python/2. Data Processing/2. Data Analysis/Initial_model_accuracy_results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sensata2com-my.sharepoint.com/personal/sofithcheallaigh_sensata_com/Documents/Desktop/Temp Git/masters_project/Python/2. Data Processing/2. Data Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\2. Data Processing\2. Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D4A59E93-1CC9-4870-80B0-3A467EC14181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{318336AC-F486-4FA6-A26B-B2F101EB6143}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F12637-CAD9-4AD8-A28C-8395C9496E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{96ABA9FB-0DD9-458B-8A8D-B7C9E47C7F0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{96ABA9FB-0DD9-458B-8A8D-B7C9E47C7F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="BinarySearch" sheetId="1" r:id="rId1"/>
     <sheet name="GridSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="32">
   <si>
     <t>Train</t>
   </si>
@@ -113,6 +114,24 @@
   </si>
   <si>
     <t>Display stand</t>
+  </si>
+  <si>
+    <t>Storage Box for both data sets</t>
+  </si>
+  <si>
+    <t>Display Stand for both data sets</t>
+  </si>
+  <si>
+    <t>Door for both data sets</t>
+  </si>
+  <si>
+    <t>Open Hallway for both data sets</t>
+  </si>
+  <si>
+    <t>Grid Wise Analysis</t>
+  </si>
+  <si>
+    <t>Full Data Set</t>
   </si>
 </sst>
 </file>
@@ -378,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -465,73 +484,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,39 +972,39 @@
       <selection activeCell="B12" sqref="B12:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="47" t="s">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="49" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="49" t="s">
+      <c r="F3" s="52"/>
+      <c r="G3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="49" t="s">
+      <c r="H3" s="52"/>
+      <c r="I3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="45" t="s">
+      <c r="J3" s="52"/>
+      <c r="K3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="46"/>
-    </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="48"/>
+      <c r="L3" s="45"/>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="53"/>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1079,7 +1106,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1114,7 +1141,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1149,7 +1176,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1184,85 +1211,85 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="51" t="s">
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="53"/>
-    </row>
-    <row r="18" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="47" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="50"/>
+    </row>
+    <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="49" t="s">
+      <c r="D18" s="52"/>
+      <c r="E18" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="50"/>
-      <c r="G18" s="49" t="s">
+      <c r="F18" s="52"/>
+      <c r="G18" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="50"/>
-      <c r="I18" s="49" t="s">
+      <c r="H18" s="52"/>
+      <c r="I18" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="50"/>
-      <c r="K18" s="49" t="s">
+      <c r="J18" s="52"/>
+      <c r="K18" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="50"/>
-      <c r="M18" s="49" t="s">
+      <c r="L18" s="52"/>
+      <c r="M18" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="50"/>
-      <c r="O18" s="49" t="s">
+      <c r="N18" s="52"/>
+      <c r="O18" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="49" t="s">
+      <c r="P18" s="52"/>
+      <c r="Q18" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="50"/>
-      <c r="S18" s="49" t="s">
+      <c r="R18" s="52"/>
+      <c r="S18" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="T18" s="50"/>
-    </row>
-    <row r="19" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="54"/>
+      <c r="T18" s="52"/>
+    </row>
+    <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="47"/>
       <c r="C19" s="30" t="s">
         <v>0</v>
       </c>
@@ -1318,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1404,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>4</v>
       </c>
@@ -1436,7 +1463,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>5</v>
       </c>
@@ -1495,7 +1522,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>6</v>
       </c>
@@ -1554,7 +1581,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>7</v>
       </c>
@@ -1613,7 +1640,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="24" t="s">
         <v>15</v>
       </c>
@@ -1672,73 +1699,73 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="51" t="s">
+    <row r="27" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="53"/>
-    </row>
-    <row r="29" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="47" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="50"/>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="49" t="s">
+      <c r="D29" s="52"/>
+      <c r="E29" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="50"/>
-      <c r="G29" s="49" t="s">
+      <c r="F29" s="52"/>
+      <c r="G29" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="49" t="s">
+      <c r="H29" s="52"/>
+      <c r="I29" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="50"/>
-      <c r="K29" s="49" t="s">
+      <c r="J29" s="52"/>
+      <c r="K29" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="50"/>
-      <c r="M29" s="49" t="s">
+      <c r="L29" s="52"/>
+      <c r="M29" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N29" s="50"/>
-      <c r="O29" s="49" t="s">
+      <c r="N29" s="52"/>
+      <c r="O29" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="P29" s="50"/>
-      <c r="Q29" s="49" t="s">
+      <c r="P29" s="52"/>
+      <c r="Q29" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="R29" s="50"/>
-      <c r="S29" s="49" t="s">
+      <c r="R29" s="52"/>
+      <c r="S29" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="T29" s="50"/>
-    </row>
-    <row r="30" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="54"/>
+      <c r="T29" s="52"/>
+    </row>
+    <row r="30" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="47"/>
       <c r="C30" s="33" t="s">
         <v>0</v>
       </c>
@@ -1794,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="22" t="s">
         <v>2</v>
       </c>
@@ -1853,7 +1880,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
         <v>4</v>
       </c>
@@ -1912,7 +1939,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1998,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
         <v>6</v>
       </c>
@@ -2030,7 +2057,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
         <v>7</v>
       </c>
@@ -2089,7 +2116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="24" t="s">
         <v>15</v>
       </c>
@@ -2148,73 +2175,73 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="51" t="s">
+    <row r="38" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="52"/>
-      <c r="S39" s="52"/>
-      <c r="T39" s="53"/>
-    </row>
-    <row r="40" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="47" t="s">
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="50"/>
+    </row>
+    <row r="40" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="49" t="s">
+      <c r="D40" s="52"/>
+      <c r="E40" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" s="49" t="s">
+      <c r="F40" s="52"/>
+      <c r="G40" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="50"/>
-      <c r="I40" s="49" t="s">
+      <c r="H40" s="52"/>
+      <c r="I40" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J40" s="50"/>
-      <c r="K40" s="49" t="s">
+      <c r="J40" s="52"/>
+      <c r="K40" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="50"/>
-      <c r="M40" s="49" t="s">
+      <c r="L40" s="52"/>
+      <c r="M40" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N40" s="50"/>
-      <c r="O40" s="49" t="s">
+      <c r="N40" s="52"/>
+      <c r="O40" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="49" t="s">
+      <c r="P40" s="52"/>
+      <c r="Q40" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="R40" s="50"/>
-      <c r="S40" s="49" t="s">
+      <c r="R40" s="52"/>
+      <c r="S40" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="T40" s="50"/>
-    </row>
-    <row r="41" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="54"/>
+      <c r="T40" s="52"/>
+    </row>
+    <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="47"/>
       <c r="C41" s="33" t="s">
         <v>0</v>
       </c>
@@ -2270,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="22" t="s">
         <v>2</v>
       </c>
@@ -2329,7 +2356,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="23" t="s">
         <v>4</v>
       </c>
@@ -2388,7 +2415,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="23" t="s">
         <v>5</v>
       </c>
@@ -2447,7 +2474,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="23" t="s">
         <v>6</v>
       </c>
@@ -2506,7 +2533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="23" t="s">
         <v>7</v>
       </c>
@@ -2565,7 +2592,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="24" t="s">
         <v>15</v>
       </c>
@@ -2624,73 +2651,73 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="50" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="51" t="s">
+    <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="52"/>
-      <c r="L50" s="52"/>
-      <c r="M50" s="52"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="52"/>
-      <c r="P50" s="52"/>
-      <c r="Q50" s="52"/>
-      <c r="R50" s="52"/>
-      <c r="S50" s="52"/>
-      <c r="T50" s="53"/>
-    </row>
-    <row r="51" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="47" t="s">
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="R50" s="49"/>
+      <c r="S50" s="49"/>
+      <c r="T50" s="50"/>
+    </row>
+    <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="50"/>
-      <c r="E51" s="49" t="s">
+      <c r="D51" s="52"/>
+      <c r="E51" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="50"/>
-      <c r="G51" s="49" t="s">
+      <c r="F51" s="52"/>
+      <c r="G51" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H51" s="50"/>
-      <c r="I51" s="49" t="s">
+      <c r="H51" s="52"/>
+      <c r="I51" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J51" s="50"/>
-      <c r="K51" s="49" t="s">
+      <c r="J51" s="52"/>
+      <c r="K51" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="L51" s="50"/>
-      <c r="M51" s="49" t="s">
+      <c r="L51" s="52"/>
+      <c r="M51" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="N51" s="50"/>
-      <c r="O51" s="49" t="s">
+      <c r="N51" s="52"/>
+      <c r="O51" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="49" t="s">
+      <c r="P51" s="52"/>
+      <c r="Q51" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="R51" s="50"/>
-      <c r="S51" s="49" t="s">
+      <c r="R51" s="52"/>
+      <c r="S51" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="T51" s="50"/>
-    </row>
-    <row r="52" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="54"/>
+      <c r="T51" s="52"/>
+    </row>
+    <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="47"/>
       <c r="C52" s="3" t="s">
         <v>0</v>
       </c>
@@ -2746,7 +2773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53" s="22" t="s">
         <v>2</v>
       </c>
@@ -2805,7 +2832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B54" s="23" t="s">
         <v>4</v>
       </c>
@@ -2864,7 +2891,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55" s="23" t="s">
         <v>5</v>
       </c>
@@ -2923,7 +2950,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56" s="23" t="s">
         <v>6</v>
       </c>
@@ -2982,7 +3009,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B57" s="23" t="s">
         <v>7</v>
       </c>
@@ -3041,7 +3068,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="24" t="s">
         <v>15</v>
       </c>
@@ -3100,72 +3127,72 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="55" t="s">
+    <row r="61" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="55"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="55"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="55"/>
-      <c r="M61" s="55"/>
-      <c r="N61" s="55"/>
-      <c r="O61" s="55"/>
-      <c r="P61" s="55"/>
-      <c r="Q61" s="55"/>
-      <c r="R61" s="55"/>
-      <c r="S61" s="55"/>
-      <c r="T61" s="55"/>
-    </row>
-    <row r="62" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="47" t="s">
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
+      <c r="I61" s="43"/>
+      <c r="J61" s="43"/>
+      <c r="K61" s="43"/>
+      <c r="L61" s="43"/>
+      <c r="M61" s="43"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
+      <c r="P61" s="43"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
+      <c r="S61" s="43"/>
+      <c r="T61" s="43"/>
+    </row>
+    <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="45" t="s">
+      <c r="C62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="46"/>
-      <c r="E62" s="45" t="s">
+      <c r="D62" s="45"/>
+      <c r="E62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="46"/>
-      <c r="G62" s="45" t="s">
+      <c r="F62" s="45"/>
+      <c r="G62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="46"/>
-      <c r="I62" s="45" t="s">
+      <c r="H62" s="45"/>
+      <c r="I62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="J62" s="46"/>
-      <c r="K62" s="45" t="s">
+      <c r="J62" s="45"/>
+      <c r="K62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="L62" s="46"/>
-      <c r="M62" s="45" t="s">
+      <c r="L62" s="45"/>
+      <c r="M62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="N62" s="46"/>
-      <c r="O62" s="45" t="s">
+      <c r="N62" s="45"/>
+      <c r="O62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="P62" s="46"/>
-      <c r="Q62" s="45" t="s">
+      <c r="P62" s="45"/>
+      <c r="Q62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="R62" s="46"/>
-      <c r="S62" s="45" t="s">
+      <c r="R62" s="45"/>
+      <c r="S62" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="T62" s="46"/>
-    </row>
-    <row r="63" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="54"/>
+      <c r="T62" s="45"/>
+    </row>
+    <row r="63" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="47"/>
       <c r="C63" s="12" t="s">
         <v>0</v>
       </c>
@@ -3221,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B64" s="22" t="s">
         <v>2</v>
       </c>
@@ -3280,7 +3307,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B65" s="23" t="s">
         <v>4</v>
       </c>
@@ -3339,7 +3366,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66" s="23" t="s">
         <v>5</v>
       </c>
@@ -3398,7 +3425,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B67" s="23" t="s">
         <v>6</v>
       </c>
@@ -3457,7 +3484,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B68" s="23" t="s">
         <v>7</v>
       </c>
@@ -3516,7 +3543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="24" t="s">
         <v>15</v>
       </c>
@@ -3577,17 +3604,40 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="B61:T61"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="S62:T62"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B17:T17"/>
+    <mergeCell ref="B28:T28"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
     <mergeCell ref="B39:T39"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:D51"/>
@@ -3604,40 +3654,17 @@
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B17:T17"/>
-    <mergeCell ref="B28:T28"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B61:T61"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="S62:T62"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="I62:J62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3648,57 +3675,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7590D5-C11D-488D-8E32-69EE70D35CC7}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="11" max="11" width="0.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="11" max="11" width="0.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="47" t="s">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="49" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="50"/>
-      <c r="G5" s="49" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="49" t="s">
+      <c r="H5" s="52"/>
+      <c r="I5" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="50"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="34" t="s">
+      <c r="J5" s="52"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="35"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="48"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="53"/>
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
@@ -3723,7 +3750,7 @@
       <c r="J6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="42"/>
+      <c r="K6" s="40"/>
       <c r="L6" s="12" t="s">
         <v>0</v>
       </c>
@@ -3731,200 +3758,200 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="34">
         <v>80</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="35">
         <v>80</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>99</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="35">
         <v>99</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="34">
         <v>97</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="35">
         <v>97</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="36">
         <v>96</v>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="35">
         <v>96</v>
       </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="36">
+      <c r="K7" s="41"/>
+      <c r="L7" s="34">
         <v>93</v>
       </c>
-      <c r="M7" s="37">
+      <c r="M7" s="35">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="36">
-        <v>100</v>
-      </c>
-      <c r="D8" s="37">
-        <v>100</v>
-      </c>
-      <c r="E8" s="36">
-        <v>100</v>
-      </c>
-      <c r="F8" s="37">
-        <v>100</v>
-      </c>
-      <c r="G8" s="36">
-        <v>100</v>
-      </c>
-      <c r="H8" s="37">
-        <v>100</v>
-      </c>
-      <c r="I8" s="38">
-        <v>100</v>
-      </c>
-      <c r="J8" s="37">
-        <v>100</v>
-      </c>
-      <c r="K8" s="43"/>
-      <c r="L8" s="36">
-        <v>100</v>
-      </c>
-      <c r="M8" s="37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C8" s="34">
+        <v>100</v>
+      </c>
+      <c r="D8" s="35">
+        <v>100</v>
+      </c>
+      <c r="E8" s="34">
+        <v>100</v>
+      </c>
+      <c r="F8" s="35">
+        <v>100</v>
+      </c>
+      <c r="G8" s="34">
+        <v>100</v>
+      </c>
+      <c r="H8" s="35">
+        <v>100</v>
+      </c>
+      <c r="I8" s="36">
+        <v>100</v>
+      </c>
+      <c r="J8" s="35">
+        <v>100</v>
+      </c>
+      <c r="K8" s="41"/>
+      <c r="L8" s="34">
+        <v>100</v>
+      </c>
+      <c r="M8" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="36">
-        <v>100</v>
-      </c>
-      <c r="D9" s="37">
-        <v>100</v>
-      </c>
-      <c r="E9" s="36">
-        <v>100</v>
-      </c>
-      <c r="F9" s="37">
-        <v>100</v>
-      </c>
-      <c r="G9" s="36">
-        <v>100</v>
-      </c>
-      <c r="H9" s="37">
-        <v>100</v>
-      </c>
-      <c r="I9" s="38">
-        <v>100</v>
-      </c>
-      <c r="J9" s="37">
-        <v>100</v>
-      </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="36">
-        <v>100</v>
-      </c>
-      <c r="M9" s="37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C9" s="34">
+        <v>100</v>
+      </c>
+      <c r="D9" s="35">
+        <v>100</v>
+      </c>
+      <c r="E9" s="34">
+        <v>100</v>
+      </c>
+      <c r="F9" s="35">
+        <v>100</v>
+      </c>
+      <c r="G9" s="34">
+        <v>100</v>
+      </c>
+      <c r="H9" s="35">
+        <v>100</v>
+      </c>
+      <c r="I9" s="36">
+        <v>100</v>
+      </c>
+      <c r="J9" s="35">
+        <v>100</v>
+      </c>
+      <c r="K9" s="41"/>
+      <c r="L9" s="34">
+        <v>100</v>
+      </c>
+      <c r="M9" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="34">
         <v>66</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="35">
         <v>65</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>97</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="35">
         <v>97</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="34">
         <v>96</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="35">
         <v>96</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="36">
         <v>95</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="35">
         <v>95</v>
       </c>
-      <c r="K10" s="43"/>
-      <c r="L10" s="36">
+      <c r="K10" s="41"/>
+      <c r="L10" s="34">
         <v>95</v>
       </c>
-      <c r="M10" s="37">
+      <c r="M10" s="35">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="37">
         <v>91</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="38">
         <v>91</v>
       </c>
-      <c r="E11" s="39">
-        <v>100</v>
-      </c>
-      <c r="F11" s="40">
-        <v>100</v>
-      </c>
-      <c r="G11" s="39">
+      <c r="E11" s="37">
+        <v>100</v>
+      </c>
+      <c r="F11" s="38">
+        <v>100</v>
+      </c>
+      <c r="G11" s="37">
         <v>99</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="38">
         <v>99</v>
       </c>
-      <c r="I11" s="41">
+      <c r="I11" s="39">
         <v>99</v>
       </c>
-      <c r="J11" s="40">
-        <v>100</v>
-      </c>
-      <c r="K11" s="44"/>
-      <c r="L11" s="39">
+      <c r="J11" s="38">
+        <v>100</v>
+      </c>
+      <c r="K11" s="42"/>
+      <c r="L11" s="37">
         <v>97</v>
       </c>
-      <c r="M11" s="40">
+      <c r="M11" s="38">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="56" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="34">
         <v>97</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="35">
         <v>97</v>
       </c>
-      <c r="E12" s="36">
-        <v>100</v>
-      </c>
-      <c r="F12" s="37">
+      <c r="E12" s="34">
+        <v>100</v>
+      </c>
+      <c r="F12" s="35">
         <v>100</v>
       </c>
     </row>
@@ -3987,4 +4014,474 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8826DE36-56A1-4A78-90D6-9C7F29B3C60A}">
+  <dimension ref="B2:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="58"/>
+    </row>
+    <row r="4" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="55"/>
+      <c r="E4" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="55"/>
+      <c r="G4" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="55"/>
+      <c r="I4" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="55"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="53"/>
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="34">
+        <v>90</v>
+      </c>
+      <c r="D6" s="35">
+        <v>90</v>
+      </c>
+      <c r="E6" s="34">
+        <v>80</v>
+      </c>
+      <c r="F6" s="35">
+        <v>79</v>
+      </c>
+      <c r="G6" s="34">
+        <v>90</v>
+      </c>
+      <c r="H6" s="35">
+        <v>90</v>
+      </c>
+      <c r="I6" s="34">
+        <v>76</v>
+      </c>
+      <c r="J6" s="35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="34">
+        <v>90</v>
+      </c>
+      <c r="D7" s="35">
+        <v>89</v>
+      </c>
+      <c r="E7" s="34">
+        <v>91</v>
+      </c>
+      <c r="F7" s="35">
+        <v>88</v>
+      </c>
+      <c r="G7" s="34">
+        <v>90</v>
+      </c>
+      <c r="H7" s="35">
+        <v>90</v>
+      </c>
+      <c r="I7" s="34">
+        <v>89</v>
+      </c>
+      <c r="J7" s="35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="34">
+        <v>89</v>
+      </c>
+      <c r="D8" s="35">
+        <v>88</v>
+      </c>
+      <c r="E8" s="34">
+        <v>90</v>
+      </c>
+      <c r="F8" s="35">
+        <v>88</v>
+      </c>
+      <c r="G8" s="34">
+        <v>89</v>
+      </c>
+      <c r="H8" s="35">
+        <v>89</v>
+      </c>
+      <c r="I8" s="34">
+        <v>88</v>
+      </c>
+      <c r="J8" s="35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="34">
+        <v>90</v>
+      </c>
+      <c r="D9" s="35">
+        <v>90</v>
+      </c>
+      <c r="E9" s="34">
+        <v>88</v>
+      </c>
+      <c r="F9" s="35">
+        <v>88</v>
+      </c>
+      <c r="G9" s="34">
+        <v>90</v>
+      </c>
+      <c r="H9" s="35">
+        <v>90</v>
+      </c>
+      <c r="I9" s="34">
+        <v>75</v>
+      </c>
+      <c r="J9" s="35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="37">
+        <v>90</v>
+      </c>
+      <c r="D10" s="38">
+        <v>90</v>
+      </c>
+      <c r="E10" s="37">
+        <v>90</v>
+      </c>
+      <c r="F10" s="38">
+        <v>90</v>
+      </c>
+      <c r="G10" s="37">
+        <v>90</v>
+      </c>
+      <c r="H10" s="38">
+        <v>90</v>
+      </c>
+      <c r="I10" s="37">
+        <v>79</v>
+      </c>
+      <c r="J10" s="38">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="58"/>
+    </row>
+    <row r="14" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="55"/>
+      <c r="E14" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="55"/>
+      <c r="G14" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="55"/>
+      <c r="I14" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="55"/>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="53"/>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="34">
+        <v>50</v>
+      </c>
+      <c r="D16" s="35">
+        <v>50</v>
+      </c>
+      <c r="E16" s="34">
+        <v>50</v>
+      </c>
+      <c r="F16" s="35">
+        <v>50</v>
+      </c>
+      <c r="G16" s="34">
+        <v>50</v>
+      </c>
+      <c r="H16" s="35">
+        <v>50</v>
+      </c>
+      <c r="I16" s="34">
+        <v>50</v>
+      </c>
+      <c r="J16" s="35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="34">
+        <v>52</v>
+      </c>
+      <c r="D17" s="35">
+        <v>45</v>
+      </c>
+      <c r="E17" s="34">
+        <v>53</v>
+      </c>
+      <c r="F17" s="35">
+        <v>40</v>
+      </c>
+      <c r="G17" s="34">
+        <v>51</v>
+      </c>
+      <c r="H17" s="35">
+        <v>48</v>
+      </c>
+      <c r="I17" s="34">
+        <v>55</v>
+      </c>
+      <c r="J17" s="35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="34">
+        <v>50</v>
+      </c>
+      <c r="D18" s="35">
+        <v>49</v>
+      </c>
+      <c r="E18" s="34">
+        <v>51</v>
+      </c>
+      <c r="F18" s="35">
+        <v>46</v>
+      </c>
+      <c r="G18" s="34">
+        <v>50</v>
+      </c>
+      <c r="H18" s="35">
+        <v>50</v>
+      </c>
+      <c r="I18" s="34">
+        <v>53</v>
+      </c>
+      <c r="J18" s="35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="34">
+        <v>50</v>
+      </c>
+      <c r="D19" s="35">
+        <v>50</v>
+      </c>
+      <c r="E19" s="34">
+        <v>50</v>
+      </c>
+      <c r="F19" s="35">
+        <v>50</v>
+      </c>
+      <c r="G19" s="34">
+        <v>50</v>
+      </c>
+      <c r="H19" s="35">
+        <v>50</v>
+      </c>
+      <c r="I19" s="34">
+        <v>50</v>
+      </c>
+      <c r="J19" s="35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="37">
+        <v>50</v>
+      </c>
+      <c r="D20" s="38">
+        <v>50</v>
+      </c>
+      <c r="E20" s="37">
+        <v>50</v>
+      </c>
+      <c r="F20" s="38">
+        <v>50</v>
+      </c>
+      <c r="G20" s="37">
+        <v>50</v>
+      </c>
+      <c r="H20" s="38">
+        <v>50</v>
+      </c>
+      <c r="I20" s="37">
+        <v>50</v>
+      </c>
+      <c r="J20" s="38">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="B3:J3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C6:J10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:J20">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating model accuracy sheet
</commit_message>
<xml_diff>
--- a/Python/2. Data Processing/2. Data Analysis/Initial_model_accuracy_results.xlsx
+++ b/Python/2. Data Processing/2. Data Analysis/Initial_model_accuracy_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Courses\UUJ\Research Project\masters_project\Python\2. Data Processing\2. Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F12637-CAD9-4AD8-A28C-8395C9496E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625ABE22-69B9-43B4-8E32-E9C268ABA350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{96ABA9FB-0DD9-458B-8A8D-B7C9E47C7F0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{96ABA9FB-0DD9-458B-8A8D-B7C9E47C7F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="BinarySearch" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +178,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -393,11 +399,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -490,18 +524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,37 +539,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -550,14 +587,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,16 +640,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>430306</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>35860</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>239806</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>102535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>535691</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>121814</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>345191</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>178964</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -612,8 +672,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9036424" y="762001"/>
-          <a:ext cx="4372585" cy="1547201"/>
+          <a:off x="10631581" y="674035"/>
+          <a:ext cx="4372585" cy="1638529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -625,15 +685,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>417195</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>445008</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>159449</xdr:rowOff>
+      <xdr:colOff>435483</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>130874</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -656,8 +716,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1036320" y="2933700"/>
-          <a:ext cx="6144768" cy="4388549"/>
+          <a:off x="1026795" y="3217545"/>
+          <a:ext cx="6095238" cy="4571429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -979,32 +1039,32 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="51" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="52"/>
-      <c r="G3" s="51" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="51" t="s">
+      <c r="H3" s="46"/>
+      <c r="I3" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="44" t="s">
+      <c r="J3" s="46"/>
+      <c r="K3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="45"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="53"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1225,71 +1285,71 @@
     </row>
     <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="49"/>
-      <c r="R17" s="49"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="50"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="49"/>
     </row>
     <row r="18" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="51" t="s">
+      <c r="D18" s="46"/>
+      <c r="E18" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="51" t="s">
+      <c r="F18" s="46"/>
+      <c r="G18" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="52"/>
-      <c r="I18" s="51" t="s">
+      <c r="H18" s="46"/>
+      <c r="I18" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="52"/>
-      <c r="K18" s="51" t="s">
+      <c r="J18" s="46"/>
+      <c r="K18" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="52"/>
-      <c r="M18" s="51" t="s">
+      <c r="L18" s="46"/>
+      <c r="M18" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N18" s="52"/>
-      <c r="O18" s="51" t="s">
+      <c r="N18" s="46"/>
+      <c r="O18" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="51" t="s">
+      <c r="P18" s="46"/>
+      <c r="Q18" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="52"/>
-      <c r="S18" s="51" t="s">
+      <c r="R18" s="46"/>
+      <c r="S18" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="T18" s="52"/>
+      <c r="T18" s="46"/>
     </row>
     <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="30" t="s">
         <v>0</v>
       </c>
@@ -1701,71 +1761,71 @@
     </row>
     <row r="27" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="50"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="49"/>
     </row>
     <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="52"/>
-      <c r="E29" s="51" t="s">
+      <c r="D29" s="46"/>
+      <c r="E29" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="52"/>
-      <c r="G29" s="51" t="s">
+      <c r="F29" s="46"/>
+      <c r="G29" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="52"/>
-      <c r="I29" s="51" t="s">
+      <c r="H29" s="46"/>
+      <c r="I29" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J29" s="52"/>
-      <c r="K29" s="51" t="s">
+      <c r="J29" s="46"/>
+      <c r="K29" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="52"/>
-      <c r="M29" s="51" t="s">
+      <c r="L29" s="46"/>
+      <c r="M29" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N29" s="52"/>
-      <c r="O29" s="51" t="s">
+      <c r="N29" s="46"/>
+      <c r="O29" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="P29" s="52"/>
-      <c r="Q29" s="51" t="s">
+      <c r="P29" s="46"/>
+      <c r="Q29" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="R29" s="52"/>
-      <c r="S29" s="51" t="s">
+      <c r="R29" s="46"/>
+      <c r="S29" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="T29" s="52"/>
+      <c r="T29" s="46"/>
     </row>
     <row r="30" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="47"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="33" t="s">
         <v>0</v>
       </c>
@@ -2177,71 +2237,71 @@
     </row>
     <row r="38" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="50"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="48"/>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="48"/>
+      <c r="T39" s="49"/>
     </row>
     <row r="40" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="51" t="s">
+      <c r="D40" s="46"/>
+      <c r="E40" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="52"/>
-      <c r="G40" s="51" t="s">
+      <c r="F40" s="46"/>
+      <c r="G40" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="52"/>
-      <c r="I40" s="51" t="s">
+      <c r="H40" s="46"/>
+      <c r="I40" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J40" s="52"/>
-      <c r="K40" s="51" t="s">
+      <c r="J40" s="46"/>
+      <c r="K40" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="52"/>
-      <c r="M40" s="51" t="s">
+      <c r="L40" s="46"/>
+      <c r="M40" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N40" s="52"/>
-      <c r="O40" s="51" t="s">
+      <c r="N40" s="46"/>
+      <c r="O40" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="51" t="s">
+      <c r="P40" s="46"/>
+      <c r="Q40" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="R40" s="52"/>
-      <c r="S40" s="51" t="s">
+      <c r="R40" s="46"/>
+      <c r="S40" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="T40" s="52"/>
+      <c r="T40" s="46"/>
     </row>
     <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="47"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="33" t="s">
         <v>0</v>
       </c>
@@ -2653,71 +2713,71 @@
     </row>
     <row r="49" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="48" t="s">
+      <c r="B50" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="49"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="Q50" s="49"/>
-      <c r="R50" s="49"/>
-      <c r="S50" s="49"/>
-      <c r="T50" s="50"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="48"/>
+      <c r="T50" s="49"/>
     </row>
     <row r="51" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="51" t="s">
+      <c r="C51" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="52"/>
-      <c r="E51" s="51" t="s">
+      <c r="D51" s="46"/>
+      <c r="E51" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="52"/>
-      <c r="G51" s="51" t="s">
+      <c r="F51" s="46"/>
+      <c r="G51" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H51" s="52"/>
-      <c r="I51" s="51" t="s">
+      <c r="H51" s="46"/>
+      <c r="I51" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J51" s="52"/>
-      <c r="K51" s="51" t="s">
+      <c r="J51" s="46"/>
+      <c r="K51" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="L51" s="52"/>
-      <c r="M51" s="51" t="s">
+      <c r="L51" s="46"/>
+      <c r="M51" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="N51" s="52"/>
-      <c r="O51" s="51" t="s">
+      <c r="N51" s="46"/>
+      <c r="O51" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="P51" s="52"/>
-      <c r="Q51" s="51" t="s">
+      <c r="P51" s="46"/>
+      <c r="Q51" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="R51" s="52"/>
-      <c r="S51" s="51" t="s">
+      <c r="R51" s="46"/>
+      <c r="S51" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="T51" s="52"/>
+      <c r="T51" s="46"/>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="47"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="3" t="s">
         <v>0</v>
       </c>
@@ -3128,71 +3188,71 @@
       </c>
     </row>
     <row r="61" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C61" s="43"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="43"/>
-      <c r="I61" s="43"/>
-      <c r="J61" s="43"/>
-      <c r="K61" s="43"/>
-      <c r="L61" s="43"/>
-      <c r="M61" s="43"/>
-      <c r="N61" s="43"/>
-      <c r="O61" s="43"/>
-      <c r="P61" s="43"/>
-      <c r="Q61" s="43"/>
-      <c r="R61" s="43"/>
-      <c r="S61" s="43"/>
-      <c r="T61" s="43"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="51"/>
+      <c r="L61" s="51"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="51"/>
+      <c r="O61" s="51"/>
+      <c r="P61" s="51"/>
+      <c r="Q61" s="51"/>
+      <c r="R61" s="51"/>
+      <c r="S61" s="51"/>
+      <c r="T61" s="51"/>
     </row>
     <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="46" t="s">
+      <c r="B62" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="44" t="s">
+      <c r="D62" s="42"/>
+      <c r="E62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="45"/>
-      <c r="G62" s="44" t="s">
+      <c r="F62" s="42"/>
+      <c r="G62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="45"/>
-      <c r="I62" s="44" t="s">
+      <c r="H62" s="42"/>
+      <c r="I62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="J62" s="45"/>
-      <c r="K62" s="44" t="s">
+      <c r="J62" s="42"/>
+      <c r="K62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="L62" s="45"/>
-      <c r="M62" s="44" t="s">
+      <c r="L62" s="42"/>
+      <c r="M62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="N62" s="45"/>
-      <c r="O62" s="44" t="s">
+      <c r="N62" s="42"/>
+      <c r="O62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="P62" s="45"/>
-      <c r="Q62" s="44" t="s">
+      <c r="P62" s="42"/>
+      <c r="Q62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="R62" s="45"/>
-      <c r="S62" s="44" t="s">
+      <c r="R62" s="42"/>
+      <c r="S62" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="T62" s="45"/>
+      <c r="T62" s="42"/>
     </row>
     <row r="63" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="47"/>
+      <c r="B63" s="50"/>
       <c r="C63" s="12" t="s">
         <v>0</v>
       </c>
@@ -3604,40 +3664,17 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B17:T17"/>
-    <mergeCell ref="B28:T28"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="B61:T61"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="O62:P62"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="S62:T62"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="I62:J62"/>
     <mergeCell ref="B39:T39"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:D51"/>
@@ -3654,17 +3691,40 @@
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="O40:P40"/>
     <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="B61:T61"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="O62:P62"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="S62:T62"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B17:T17"/>
+    <mergeCell ref="B28:T28"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3673,287 +3733,345 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7590D5-C11D-488D-8E32-69EE70D35CC7}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="0.7109375" customWidth="1"/>
+    <col min="12" max="12" width="0.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="46" t="s">
+      <c r="K2" s="59"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K3" s="59"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="59"/>
+      <c r="B5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="51" t="s">
+      <c r="D5" s="46"/>
+      <c r="E5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="46"/>
+      <c r="G5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="51" t="s">
+      <c r="H5" s="46"/>
+      <c r="I5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="52"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="12" t="s">
+      <c r="J5" s="46"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53"/>
-      <c r="C6" s="3" t="s">
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="59"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="33" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="59"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="59"/>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="62">
         <v>80</v>
       </c>
       <c r="D7" s="35">
         <v>80</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="64">
         <v>99</v>
       </c>
       <c r="F7" s="35">
         <v>99</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="62">
         <v>97</v>
       </c>
       <c r="H7" s="35">
         <v>97</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="62">
         <v>96</v>
       </c>
       <c r="J7" s="35">
         <v>96</v>
       </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="34">
+      <c r="K7" s="59"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="34">
         <v>93</v>
       </c>
-      <c r="M7" s="35">
+      <c r="N7" s="35">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="59"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="34">
-        <v>100</v>
-      </c>
-      <c r="D8" s="35">
-        <v>100</v>
-      </c>
-      <c r="E8" s="34">
-        <v>100</v>
-      </c>
-      <c r="F8" s="35">
-        <v>100</v>
-      </c>
-      <c r="G8" s="34">
-        <v>100</v>
-      </c>
-      <c r="H8" s="35">
-        <v>100</v>
-      </c>
-      <c r="I8" s="36">
-        <v>100</v>
-      </c>
-      <c r="J8" s="35">
-        <v>100</v>
-      </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="34">
-        <v>100</v>
-      </c>
-      <c r="M8" s="35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="65">
+        <v>100</v>
+      </c>
+      <c r="D8" s="66">
+        <v>100</v>
+      </c>
+      <c r="E8" s="65">
+        <v>100</v>
+      </c>
+      <c r="F8" s="66">
+        <v>100</v>
+      </c>
+      <c r="G8" s="65">
+        <v>100</v>
+      </c>
+      <c r="H8" s="66">
+        <v>100</v>
+      </c>
+      <c r="I8" s="65">
+        <v>100</v>
+      </c>
+      <c r="J8" s="66">
+        <v>100</v>
+      </c>
+      <c r="K8" s="59"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="34">
+        <v>100</v>
+      </c>
+      <c r="N8" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="62">
         <v>100</v>
       </c>
       <c r="D9" s="35">
         <v>100</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="62">
         <v>100</v>
       </c>
       <c r="F9" s="35">
         <v>100</v>
       </c>
-      <c r="G9" s="34">
+      <c r="G9" s="62">
         <v>100</v>
       </c>
       <c r="H9" s="35">
         <v>100</v>
       </c>
-      <c r="I9" s="36">
+      <c r="I9" s="62">
         <v>100</v>
       </c>
       <c r="J9" s="35">
         <v>100</v>
       </c>
-      <c r="K9" s="41"/>
-      <c r="L9" s="34">
-        <v>100</v>
-      </c>
-      <c r="M9" s="35">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="59"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="34">
+        <v>100</v>
+      </c>
+      <c r="N9" s="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="65">
         <v>66</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="66">
         <v>65</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="65">
         <v>97</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="66">
         <v>97</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="65">
         <v>96</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="66">
         <v>96</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="65">
         <v>95</v>
       </c>
-      <c r="J10" s="35">
+      <c r="J10" s="66">
         <v>95</v>
       </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="34">
+      <c r="K10" s="59"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="34">
         <v>95</v>
       </c>
-      <c r="M10" s="35">
+      <c r="N10" s="35">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="59"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="63">
         <v>91</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="37">
         <v>91</v>
       </c>
-      <c r="E11" s="37">
-        <v>100</v>
-      </c>
-      <c r="F11" s="38">
-        <v>100</v>
-      </c>
-      <c r="G11" s="37">
+      <c r="E11" s="63">
+        <v>100</v>
+      </c>
+      <c r="F11" s="37">
+        <v>100</v>
+      </c>
+      <c r="G11" s="63">
         <v>99</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="37">
         <v>99</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="63">
         <v>99</v>
       </c>
-      <c r="J11" s="38">
-        <v>100</v>
-      </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="37">
+      <c r="J11" s="37">
+        <v>100</v>
+      </c>
+      <c r="K11" s="59"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="36">
         <v>97</v>
       </c>
-      <c r="M11" s="38">
+      <c r="N11" s="37">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="60"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C13" s="34">
         <v>97</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D13" s="35">
         <v>97</v>
       </c>
-      <c r="E12" s="34">
-        <v>100</v>
-      </c>
-      <c r="F12" s="35">
-        <v>100</v>
-      </c>
+      <c r="E13" s="34">
+        <v>100</v>
+      </c>
+      <c r="F13" s="35">
+        <v>100</v>
+      </c>
+      <c r="K13" s="59"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
+      <c r="K14" s="59"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K15" s="59"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K16" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3963,7 +4081,7 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:J11 C12:F12">
+  <conditionalFormatting sqref="C7:K12 C13:F13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3975,7 +4093,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:M11">
+  <conditionalFormatting sqref="M7:N12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3987,7 +4105,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:J11 D12:F12">
+  <conditionalFormatting sqref="D7:K12 D13:F13">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3999,7 +4117,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:M11 C12:F12">
+  <conditionalFormatting sqref="C7:N12 C13:F13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4020,7 +4138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8826DE36-56A1-4A78-90D6-9C7F29B3C60A}">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -4031,41 +4149,41 @@
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="58"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="54" t="s">
+      <c r="D4" s="56"/>
+      <c r="E4" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="54" t="s">
+      <c r="F4" s="56"/>
+      <c r="G4" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="54" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="55"/>
+      <c r="J4" s="56"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="53"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
@@ -4211,68 +4329,68 @@
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="36">
         <v>90</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="37">
         <v>90</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="36">
         <v>90</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="37">
         <v>90</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="36">
         <v>90</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="37">
         <v>90</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="36">
         <v>79</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="37">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="58"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
     </row>
     <row r="14" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="54" t="s">
+      <c r="D14" s="56"/>
+      <c r="E14" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="54" t="s">
+      <c r="F14" s="56"/>
+      <c r="G14" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="55"/>
-      <c r="I14" s="54" t="s">
+      <c r="H14" s="56"/>
+      <c r="I14" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="56"/>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="53"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
@@ -4418,45 +4536,45 @@
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="36">
         <v>50</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="37">
         <v>50</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="36">
         <v>50</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="37">
         <v>50</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="36">
         <v>50</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="37">
         <v>50</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I20" s="36">
         <v>50</v>
       </c>
-      <c r="J20" s="38">
+      <c r="J20" s="37">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B13:J13"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="B3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:J10">
     <cfRule type="colorScale" priority="2">

</xml_diff>